<commit_message>
Improve login validation and error handling; enhance sandbox creation checks and feedback; update upload functionality for better user guidance
</commit_message>
<xml_diff>
--- a/template/Curiculum.xlsx
+++ b/template/Curiculum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Programs\Scheduling Program\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Programs\SchedulingProgram3.0\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4323AE-C193-48DF-80CE-6834BADBB827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3DE3B7-BE8A-4364-939C-88DBC5C8505D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Prerequisites</t>
   </si>
   <si>
-    <t>Co-requisites</t>
-  </si>
-  <si>
     <t>Care Taker</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>MATH165, MATH166</t>
+  </si>
+  <si>
+    <t>Co_requisites</t>
   </si>
 </sst>
 </file>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="96.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,13 +456,13 @@
     <col min="4" max="4" width="93.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
     <col min="8" max="8" width="45.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="44" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,10 +488,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
@@ -502,10 +502,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="7">
         <v>3.75</v>
@@ -515,11 +515,11 @@
         <v>3</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">

</xml_diff>